<commit_message>
manually extract text of r071, r147 and replace r075 with correct paper pdf
</commit_message>
<xml_diff>
--- a/data/ReferenceErrorDetection_data.xlsx
+++ b/data/ReferenceErrorDetection_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6b78b8e360351019/_Dokumente/Studium/Master/Masterarbeit/_citation-verification/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_65A930B0D360D172BBDA3D11595ED87656C46049" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D63151D-E14E-4F85-991A-70CA9655508D}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_65A930B0D360D172BBDA3D11595ED87656C46049" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55320F08-73EB-4D51-8E6B-969425D94F0E}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5025" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5878,14 +5878,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
-      <selection activeCell="K219" sqref="K219"/>
+    <sheetView tabSelected="1" topLeftCell="B58" workbookViewId="0">
+      <selection activeCell="K76" sqref="K76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="54.85546875" customWidth="1"/>
+    <col min="10" max="10" width="26" customWidth="1"/>
     <col min="11" max="11" width="63.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" customWidth="1"/>
+    <col min="15" max="15" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
new annotation of whole Zhang dataset started
</commit_message>
<xml_diff>
--- a/data/ReferenceErrorDetection_data.xlsx
+++ b/data/ReferenceErrorDetection_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6b78b8e360351019/_Dokumente/Studium/Master/Masterarbeit/_citation-verification/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="11_65A930B0D360D172BBDA3D11595ED87656C46049" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55320F08-73EB-4D51-8E6B-969425D94F0E}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="11_65A930B0D360D172BBDA3D11595ED87656C46049" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4477FF26-5A74-40AF-A3D5-441B043CB5AD}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5878,13 +5878,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B58" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K76" sqref="K76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="54.85546875" customWidth="1"/>
+    <col min="4" max="4" width="70.5703125" customWidth="1"/>
     <col min="10" max="10" width="26" customWidth="1"/>
     <col min="11" max="11" width="63.85546875" customWidth="1"/>
     <col min="13" max="13" width="12.140625" customWidth="1"/>

</xml_diff>